<commit_message>
Implementation of initial AJAX handlers and dialogs
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Code</t>
   </si>
@@ -76,6 +76,21 @@
   </si>
   <si>
     <t>Information</t>
+  </si>
+  <si>
+    <t>message_10022_person_record_deleted_successfully</t>
+  </si>
+  <si>
+    <t>message_10023_person_multiple_records_deleted_successfully</t>
+  </si>
+  <si>
+    <t>message_10008_ajax_login_successful</t>
+  </si>
+  <si>
+    <t>message_10010_invalid_datetime_format</t>
+  </si>
+  <si>
+    <t>message_10011_expired_session_renewed</t>
   </si>
 </sst>
 </file>
@@ -393,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -510,6 +525,12 @@
       <c r="A10">
         <v>10008</v>
       </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
@@ -526,11 +547,23 @@
       <c r="A12">
         <v>10010</v>
       </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10011</v>
       </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
@@ -591,6 +624,28 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>10022</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>10023</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial implementation of Doctrine 2 ORM
Removed 'Models' namespace from Tranquility library
Modified database and session configuration to make use of table
namespaces
Removed unused dependency on lavary-menu package
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Code</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>message_10011_expired_session_renewed</t>
+  </si>
+  <si>
+    <t>message_10012_invalid_user_assigned_to_audit_trail</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -569,6 +572,12 @@
       <c r="A14">
         <v>10012</v>
       </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">

</xml_diff>

<commit_message>
Initial commit of user management screens and codebase cleanup
* Cleaned up unused event listeners
* Changed ServiceResponse::getFirstContentItem() to return null if there
are no content items
* Extended laravelcollective/form package to generate select elements
from reference data tables
* Shifted registration custom session handler into
ApplicationServiceProvider class
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Code</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>message_10012_invalid_user_assigned_to_audit_trail</t>
+  </si>
+  <si>
+    <t>message_10030_user_record_created_successfully</t>
+  </si>
+  <si>
+    <t>message_10031_user_record_updated_successfully</t>
+  </si>
+  <si>
+    <t>message_10032_user_record_deleted_successfully</t>
   </si>
 </sst>
 </file>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -658,6 +667,84 @@
         <v>11</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>10024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>10025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>10026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>10027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>10028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>10029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>10030</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>10031</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>10032</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>10033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>10034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>10035</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial implementation of 'change password' functionality
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Code</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>message_10032_user_record_deleted_successfully</t>
+  </si>
+  <si>
+    <t>message_10034_user_viewing_own_record</t>
+  </si>
+  <si>
+    <t>message_10035_password_not_long_enough</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -739,10 +745,22 @@
       <c r="A36">
         <v>10034</v>
       </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>10035</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Functionality for adding a new physical address
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Code</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>message_10035_password_not_long_enough</t>
+  </si>
+  <si>
+    <t>message_10040_physical_address_record_created_successfully</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -763,6 +766,37 @@
         <v>6</v>
       </c>
     </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>10036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>10037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>10038</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>10039</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>10040</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Shifted remainder of address functionality into own controller
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Code</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>message_10040_physical_address_record_created_successfully</t>
+  </si>
+  <si>
+    <t>message_10041_physical_address_record_updated_successfully</t>
+  </si>
+  <si>
+    <t>message_10042_physical_address_record_deleted_successfully</t>
   </si>
 </sst>
 </file>
@@ -429,18 +435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -465,7 +471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10001</v>
       </c>
@@ -476,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10002</v>
       </c>
@@ -487,7 +493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10003</v>
       </c>
@@ -498,7 +504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10004</v>
       </c>
@@ -509,7 +515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10005</v>
       </c>
@@ -520,7 +526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10006</v>
       </c>
@@ -531,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10007</v>
       </c>
@@ -542,7 +548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10008</v>
       </c>
@@ -553,7 +559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10009</v>
       </c>
@@ -564,7 +570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10010</v>
       </c>
@@ -575,7 +581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10011</v>
       </c>
@@ -586,7 +592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10012</v>
       </c>
@@ -597,42 +603,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10013</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10014</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10015</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10016</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10017</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10018</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10019</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10020</v>
       </c>
@@ -643,7 +649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10021</v>
       </c>
@@ -654,7 +660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10022</v>
       </c>
@@ -665,7 +671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10023</v>
       </c>
@@ -676,37 +682,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10024</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10025</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10026</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10027</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10028</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10029</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10030</v>
       </c>
@@ -717,7 +723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10031</v>
       </c>
@@ -728,7 +734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10032</v>
       </c>
@@ -739,12 +745,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10033</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10034</v>
       </c>
@@ -755,7 +761,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10035</v>
       </c>
@@ -766,27 +772,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10036</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10037</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10038</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10039</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>10040</v>
       </c>
@@ -794,6 +800,28 @@
         <v>30</v>
       </c>
       <c r="D42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>10041</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>10042</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed transfer of address functionality into separate controller
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>Code</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>message_10042_physical_address_record_deleted_successfully</t>
+  </si>
+  <si>
+    <t>message_10043_phone_address_record_created_successfully</t>
+  </si>
+  <si>
+    <t>message_10045_phone_address_record_deleted_successfully</t>
+  </si>
+  <si>
+    <t>message_10044_phone_address_record_updated_successfully</t>
+  </si>
+  <si>
+    <t>message_10046_electronic_address_record_created_successfully</t>
+  </si>
+  <si>
+    <t>message_10047_electronic_address_record_updated_successfully</t>
+  </si>
+  <si>
+    <t>message_10048_electronic_address_record_deleted_successfully</t>
   </si>
 </sst>
 </file>
@@ -435,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,6 +843,72 @@
         <v>11</v>
       </c>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>10043</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>10044</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>10045</v>
+      </c>
+      <c r="B47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>10046</v>
+      </c>
+      <c r="B48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>10047</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10048</v>
+      </c>
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Merged phone and electronic address services
UI cleanup for People controller
UI cleanup for address panels
Stylesheet changes for small viewports
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Code</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>message_10048_electronic_address_record_deleted_successfully</t>
+  </si>
+  <si>
+    <t>message_10049_phone_address_primary_contact_updated</t>
+  </si>
+  <si>
+    <t>message_10050_electronic_address_primary_contact_updated</t>
   </si>
 </sst>
 </file>
@@ -266,6 +272,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -301,6 +324,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,6 +949,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10049</v>
+      </c>
+      <c r="B51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>10050</v>
+      </c>
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Major reorganisation of data objects
Completed implementation of tagging
Linking to search still to come
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>Code</t>
   </si>
@@ -142,6 +143,15 @@
   </si>
   <si>
     <t>message_10050_electronic_address_primary_contact_updated</t>
+  </si>
+  <si>
+    <t>message_10060_new_tag_created</t>
+  </si>
+  <si>
+    <t>message_10061_tag_deleted</t>
+  </si>
+  <si>
+    <t>message_10062_tag_collection_updated</t>
   </si>
 </sst>
 </file>
@@ -493,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,6 +981,99 @@
         <v>11</v>
       </c>
     </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10051</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>10052</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>10053</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>10054</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>10055</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>10056</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>10057</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>10058</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>10059</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>10060</v>
+      </c>
+      <c r="B62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>10061</v>
+      </c>
+      <c r="B63" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>10062</v>
+      </c>
+      <c r="B64" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>10063</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>10064</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>10065</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User account creation from person details page
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Code</t>
   </si>
@@ -152,6 +151,9 @@
   </si>
   <si>
     <t>message_10062_tag_collection_updated</t>
+  </si>
+  <si>
+    <t>message_10033_user_already_exists</t>
   </si>
 </sst>
 </file>
@@ -505,16 +507,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -539,7 +541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>10001</v>
       </c>
@@ -550,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>10002</v>
       </c>
@@ -561,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>10003</v>
       </c>
@@ -572,7 +574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>10004</v>
       </c>
@@ -583,7 +585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>10005</v>
       </c>
@@ -594,7 +596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>10006</v>
       </c>
@@ -605,7 +607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>10007</v>
       </c>
@@ -616,7 +618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>10008</v>
       </c>
@@ -627,7 +629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10009</v>
       </c>
@@ -638,7 +640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10010</v>
       </c>
@@ -649,7 +651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10011</v>
       </c>
@@ -660,7 +662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>10012</v>
       </c>
@@ -671,42 +673,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>10013</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>10014</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>10015</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>10016</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>10017</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>10018</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>10019</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>10020</v>
       </c>
@@ -717,7 +719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>10021</v>
       </c>
@@ -728,7 +730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>10022</v>
       </c>
@@ -739,7 +741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>10023</v>
       </c>
@@ -750,37 +752,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>10024</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>10025</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>10026</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>10027</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>10028</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>10029</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>10030</v>
       </c>
@@ -791,7 +793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>10031</v>
       </c>
@@ -802,7 +804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>10032</v>
       </c>
@@ -813,12 +815,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>10033</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>10034</v>
       </c>
@@ -829,7 +837,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>10035</v>
       </c>
@@ -840,27 +848,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>10036</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>10037</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>10038</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>10039</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>10040</v>
       </c>
@@ -871,7 +879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>10041</v>
       </c>
@@ -882,7 +890,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>10042</v>
       </c>
@@ -893,7 +901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>10043</v>
       </c>
@@ -904,7 +912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>10044</v>
       </c>
@@ -915,7 +923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>10045</v>
       </c>
@@ -926,7 +934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>10046</v>
       </c>
@@ -937,7 +945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>10047</v>
       </c>
@@ -948,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>10048</v>
       </c>
@@ -959,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>10049</v>
       </c>
@@ -970,7 +978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>10050</v>
       </c>
@@ -981,52 +989,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>10052</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>10053</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>10054</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>10055</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>10056</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>10057</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>10058</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>10059</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>10060</v>
       </c>
@@ -1037,7 +1045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>10061</v>
       </c>
@@ -1048,7 +1056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>10062</v>
       </c>
@@ -1059,17 +1067,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>10063</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>10064</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>10065</v>
       </c>

</xml_diff>

<commit_message>
Implemented delete for single users
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>Code</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>message_10033_user_already_exists</t>
+  </si>
+  <si>
+    <t>message_10037_user_cannot_delete_own_record</t>
+  </si>
+  <si>
+    <t>message_10036_password_updated_successfully</t>
+  </si>
+  <si>
+    <t>message_10051_email_address_format_invalid</t>
+  </si>
+  <si>
+    <t>message_10038_username_not_available</t>
   </si>
 </sst>
 </file>
@@ -507,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -852,16 +864,34 @@
       <c r="A38">
         <v>10036</v>
       </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>10037</v>
       </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>10038</v>
       </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41">
@@ -992,6 +1022,12 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>10051</v>
+      </c>
+      <c r="B53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Initial account implementation (in progress)
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>Code</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>message_10038_username_not_available</t>
+  </si>
+  <si>
+    <t>message_10070_account_record_created_successfully</t>
+  </si>
+  <si>
+    <t>message_10071_account_record_updated_successfully</t>
+  </si>
+  <si>
+    <t>message_10072_account_record_deleted_successfully</t>
+  </si>
+  <si>
+    <t>message_10073_account_multiple_records_deleted_successfully</t>
   </si>
 </sst>
 </file>
@@ -517,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1103,19 +1115,303 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>10063</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>10064</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>10065</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>10066</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>10067</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>10068</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>10069</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>10070</v>
+      </c>
+      <c r="B72" t="s">
+        <v>49</v>
+      </c>
+      <c r="D72" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>10071</v>
+      </c>
+      <c r="B73" t="s">
+        <v>50</v>
+      </c>
+      <c r="D73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>10072</v>
+      </c>
+      <c r="B74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>10073</v>
+      </c>
+      <c r="B75" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>10074</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>10075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>10076</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>10077</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>10078</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>10079</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>10080</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>10081</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>10082</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>10083</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>10084</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>10085</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>10086</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>10087</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>10088</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>10089</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>10090</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>10091</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>10092</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>10093</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>10094</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>10095</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>10096</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>10097</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>10098</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>10099</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>10101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>10102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>10103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>10104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>10105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>10106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>10107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>10108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>10109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>10110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>10111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>10112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>10113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>10114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>10115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>10116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>10117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reworked user account updates to be handled by AJAX, as well as standard page
</commit_message>
<xml_diff>
--- a/docs/Error codes.xlsx
+++ b/docs/Error codes.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>Code</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>message_10073_account_multiple_records_deleted_successfully</t>
+  </si>
+  <si>
+    <t>message_10052_address_already_exists</t>
   </si>
 </sst>
 </file>
@@ -531,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1046,6 +1049,12 @@
       <c r="A54">
         <v>10052</v>
       </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55">

</xml_diff>